<commit_message>
Update Debug Interface + Configuration.h
</commit_message>
<xml_diff>
--- a/Electronic/Components/Electronics-Components-Index.xlsx
+++ b/Electronic/Components/Electronics-Components-Index.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="423">
   <si>
     <t>Catégorie</t>
   </si>
@@ -763,12 +763,6 @@
     <t>PCB Extension Camera Raspi</t>
   </si>
   <si>
-    <t>BluePill STM32</t>
-  </si>
-  <si>
-    <t>STM32F103C8T6 small Dev board</t>
-  </si>
-  <si>
     <t>VERSION\E-0023</t>
   </si>
   <si>
@@ -1265,6 +1259,42 @@
   </si>
   <si>
     <t>541-1.6KGTR-ND</t>
+  </si>
+  <si>
+    <t>STM32F103C8T6  IC</t>
+  </si>
+  <si>
+    <t>STM32F103</t>
+  </si>
+  <si>
+    <t>497-6063-ND</t>
+  </si>
+  <si>
+    <t>Micro USB connector</t>
+  </si>
+  <si>
+    <t>Red LED 0603 SMD</t>
+  </si>
+  <si>
+    <t>LCD Cape BeagleBone Black</t>
+  </si>
+  <si>
+    <t>LCD Cape + Max485 for BeagleBone Black</t>
+  </si>
+  <si>
+    <t>PCB Drive Motor</t>
+  </si>
+  <si>
+    <t>PCB Drive motor for 6DOF Robotic Arm</t>
+  </si>
+  <si>
+    <t>Emile Renaud / Luka Bouchard</t>
+  </si>
+  <si>
+    <t>Priceless</t>
+  </si>
+  <si>
+    <t>Jumper 2 POS</t>
   </si>
 </sst>
 </file>
@@ -1408,13 +1438,13 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1893,8 +1923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I55" sqref="I55"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1916,18 +1946,18 @@
       <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -1950,18 +1980,18 @@
       <c r="A3" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="11"/>
@@ -2645,20 +2675,20 @@
         <v>233</v>
       </c>
       <c r="D25" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="F25" s="6" t="s">
         <v>326</v>
-      </c>
-      <c r="E25" s="12" t="s">
-        <v>327</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>328</v>
       </c>
       <c r="G25" s="6"/>
       <c r="H25" s="13" t="s">
         <v>236</v>
       </c>
       <c r="I25" s="24" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="J25" s="18">
         <v>1.32</v>
@@ -2746,29 +2776,29 @@
         <v>58</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>5</v>
+        <v>142</v>
       </c>
       <c r="D28" s="23" t="s">
-        <v>245</v>
+        <v>412</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>246</v>
+        <v>411</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>235</v>
+        <v>152</v>
       </c>
       <c r="G28" s="6"/>
       <c r="H28" s="13" t="s">
-        <v>247</v>
-      </c>
-      <c r="I28" s="6" t="s">
-        <v>235</v>
+        <v>245</v>
+      </c>
+      <c r="I28" s="13" t="s">
+        <v>413</v>
       </c>
       <c r="J28" s="18">
-        <v>0</v>
+        <v>8.02</v>
       </c>
       <c r="K28" s="20">
         <v>1163842</v>
@@ -2789,20 +2819,20 @@
         <v>133</v>
       </c>
       <c r="D29" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="F29" s="6" t="s">
         <v>248</v>
-      </c>
-      <c r="E29" s="12" t="s">
-        <v>249</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>250</v>
       </c>
       <c r="G29" s="6"/>
       <c r="H29" s="13" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="J29" s="18">
         <v>0.16</v>
@@ -2822,20 +2852,20 @@
         <v>133</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G30" s="6"/>
       <c r="H30" s="24" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I30" s="13" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="J30" s="18">
         <v>0.16</v>
@@ -2855,20 +2885,20 @@
         <v>133</v>
       </c>
       <c r="D31" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>252</v>
+      </c>
+      <c r="F31" s="6" t="s">
         <v>253</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>254</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>255</v>
       </c>
       <c r="G31" s="6"/>
       <c r="H31" s="13" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="I31" s="13" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="J31" s="18">
         <v>0.16</v>
@@ -2888,20 +2918,20 @@
         <v>133</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G32" s="6"/>
       <c r="H32" s="13" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="I32" s="13" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="J32" s="19">
         <v>0.16</v>
@@ -2921,20 +2951,20 @@
         <v>133</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G33" s="6"/>
       <c r="H33" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="I33" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="J33" s="18">
         <v>0.16</v>
@@ -2954,20 +2984,20 @@
         <v>133</v>
       </c>
       <c r="D34" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="F34" s="6" t="s">
         <v>270</v>
-      </c>
-      <c r="E34" s="12" t="s">
-        <v>271</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>272</v>
       </c>
       <c r="G34" s="6"/>
       <c r="H34" s="13" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="I34" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="J34" s="18">
         <v>0.16</v>
@@ -2987,20 +3017,20 @@
         <v>133</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="G35" s="6"/>
       <c r="H35" s="13" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="I35" s="13" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="J35" s="18">
         <v>0.16</v>
@@ -3020,20 +3050,20 @@
         <v>133</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G36" s="6"/>
       <c r="H36" s="13" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="I36" s="13" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="J36" s="18">
         <v>0.16</v>
@@ -3053,20 +3083,20 @@
         <v>133</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="G37" s="6"/>
       <c r="H37" s="13" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="I37" s="13" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="J37" s="18">
         <v>0.16</v>
@@ -3086,20 +3116,20 @@
         <v>135</v>
       </c>
       <c r="D38" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="F38" s="6" t="s">
         <v>287</v>
-      </c>
-      <c r="E38" s="12" t="s">
-        <v>288</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>289</v>
       </c>
       <c r="G38" s="6"/>
       <c r="H38" s="13" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="I38" s="13" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="J38" s="18">
         <v>0.15</v>
@@ -3119,20 +3149,20 @@
         <v>135</v>
       </c>
       <c r="D39" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>291</v>
+      </c>
+      <c r="F39" s="6" t="s">
         <v>292</v>
-      </c>
-      <c r="E39" s="12" t="s">
-        <v>293</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>294</v>
       </c>
       <c r="G39" s="6"/>
       <c r="H39" s="13" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="I39" s="13" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J39" s="18">
         <v>0.15</v>
@@ -3152,20 +3182,20 @@
         <v>135</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="G40" s="6"/>
       <c r="H40" s="24" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="I40" s="13" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="J40" s="18">
         <v>0.18</v>
@@ -3185,20 +3215,20 @@
         <v>138</v>
       </c>
       <c r="D41" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>301</v>
+      </c>
+      <c r="F41" s="6" t="s">
         <v>302</v>
-      </c>
-      <c r="E41" s="12" t="s">
-        <v>303</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>304</v>
       </c>
       <c r="G41" s="6"/>
       <c r="H41" s="13" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="I41" s="13" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="J41" s="18">
         <v>0.21</v>
@@ -3218,20 +3248,20 @@
         <v>171</v>
       </c>
       <c r="D42" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>305</v>
+      </c>
+      <c r="F42" s="6" t="s">
         <v>306</v>
-      </c>
-      <c r="E42" s="12" t="s">
-        <v>307</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>308</v>
       </c>
       <c r="G42" s="6"/>
       <c r="H42" s="13" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="I42" s="13" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="J42" s="18">
         <v>0.76</v>
@@ -3251,20 +3281,20 @@
         <v>138</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G43" s="13"/>
       <c r="H43" s="13" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="I43" s="26" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="J43" s="18">
         <v>0.5</v>
@@ -3284,20 +3314,20 @@
         <v>142</v>
       </c>
       <c r="D44" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="E44" s="12" t="s">
+        <v>329</v>
+      </c>
+      <c r="F44" s="6" t="s">
         <v>330</v>
-      </c>
-      <c r="E44" s="12" t="s">
-        <v>331</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>332</v>
       </c>
       <c r="G44" s="13"/>
       <c r="H44" s="13" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="I44" s="13" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="J44" s="18">
         <v>5.0999999999999996</v>
@@ -3317,20 +3347,20 @@
         <v>139</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G45" s="6"/>
       <c r="H45" s="13" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I45" s="13" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="J45" s="18">
         <v>0.6</v>
@@ -3350,20 +3380,20 @@
         <v>135</v>
       </c>
       <c r="D46" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="E46" s="12" t="s">
+        <v>345</v>
+      </c>
+      <c r="F46" s="6" t="s">
         <v>346</v>
-      </c>
-      <c r="E46" s="12" t="s">
-        <v>347</v>
-      </c>
-      <c r="F46" s="6" t="s">
-        <v>348</v>
       </c>
       <c r="G46" s="6"/>
       <c r="H46" s="13" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="I46" s="13" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="J46" s="18">
         <v>0.15</v>
@@ -3383,20 +3413,20 @@
         <v>135</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="G47" s="6"/>
       <c r="H47" s="13" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="I47" s="13" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="J47" s="18">
         <v>0.15</v>
@@ -3416,20 +3446,20 @@
         <v>135</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="G48" s="6"/>
       <c r="H48" s="13" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="I48" s="13" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="J48" s="18">
         <v>0.28999999999999998</v>
@@ -3449,20 +3479,20 @@
         <v>133</v>
       </c>
       <c r="D49" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="E49" s="12" t="s">
+        <v>356</v>
+      </c>
+      <c r="F49" s="6" t="s">
         <v>357</v>
-      </c>
-      <c r="E49" s="12" t="s">
-        <v>358</v>
-      </c>
-      <c r="F49" s="6" t="s">
-        <v>359</v>
       </c>
       <c r="G49" s="6"/>
       <c r="H49" s="13" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="I49" s="13" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="J49" s="18">
         <v>0.47</v>
@@ -3482,20 +3512,20 @@
         <v>133</v>
       </c>
       <c r="D50" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="E50" s="12" t="s">
+        <v>359</v>
+      </c>
+      <c r="F50" s="6" t="s">
         <v>360</v>
-      </c>
-      <c r="E50" s="12" t="s">
-        <v>361</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>362</v>
       </c>
       <c r="G50" s="6"/>
       <c r="H50" s="13" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="I50" s="13" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="J50" s="18">
         <v>0.16</v>
@@ -3515,20 +3545,20 @@
         <v>141</v>
       </c>
       <c r="D51" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="E51" s="12" t="s">
+        <v>396</v>
+      </c>
+      <c r="F51" s="6" t="s">
         <v>397</v>
-      </c>
-      <c r="E51" s="12" t="s">
-        <v>398</v>
-      </c>
-      <c r="F51" s="6" t="s">
-        <v>399</v>
       </c>
       <c r="G51" s="6"/>
       <c r="H51" s="13" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="I51" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="J51" s="18">
         <v>0.27</v>
@@ -3547,21 +3577,21 @@
       <c r="C52" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="D52" s="29">
+      <c r="D52" s="27">
         <v>61300211121</v>
       </c>
       <c r="E52" s="12" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G52" s="6"/>
       <c r="H52" s="13" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="I52" s="13" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="J52" s="18">
         <v>0.2</v>
@@ -3584,17 +3614,17 @@
         <v>61300411121</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G53" s="6"/>
       <c r="H53" s="13" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="I53" s="13" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="J53" s="18">
         <v>0.27</v>
@@ -3614,20 +3644,20 @@
         <v>171</v>
       </c>
       <c r="D54" s="6" t="s">
+        <v>403</v>
+      </c>
+      <c r="E54" s="12" t="s">
+        <v>404</v>
+      </c>
+      <c r="F54" s="6" t="s">
         <v>405</v>
-      </c>
-      <c r="E54" s="12" t="s">
-        <v>406</v>
-      </c>
-      <c r="F54" s="6" t="s">
-        <v>407</v>
       </c>
       <c r="G54" s="6"/>
       <c r="H54" s="13" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="I54" s="13" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="J54" s="18">
         <v>0.73</v>
@@ -3647,20 +3677,20 @@
         <v>133</v>
       </c>
       <c r="D55" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="E55" s="12" t="s">
+        <v>408</v>
+      </c>
+      <c r="F55" s="6" t="s">
         <v>409</v>
-      </c>
-      <c r="E55" s="12" t="s">
-        <v>410</v>
-      </c>
-      <c r="F55" s="6" t="s">
-        <v>411</v>
       </c>
       <c r="G55" s="6"/>
       <c r="H55" s="13" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="I55" s="24" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="J55" s="18">
         <v>0.16</v>
@@ -3673,14 +3703,20 @@
       <c r="A56" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="B56" s="6"/>
-      <c r="C56" s="6"/>
+      <c r="B56" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>171</v>
+      </c>
       <c r="D56" s="6"/>
-      <c r="E56" s="12"/>
+      <c r="E56" s="12" t="s">
+        <v>414</v>
+      </c>
       <c r="F56" s="6"/>
       <c r="G56" s="6"/>
       <c r="H56" s="13" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="I56" s="6"/>
       <c r="J56" s="18"/>
@@ -3692,14 +3728,20 @@
       <c r="A57" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B57" s="6"/>
-      <c r="C57" s="6"/>
+      <c r="B57" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>138</v>
+      </c>
       <c r="D57" s="6"/>
-      <c r="E57" s="12"/>
+      <c r="E57" s="12" t="s">
+        <v>415</v>
+      </c>
       <c r="F57" s="6"/>
       <c r="G57" s="6"/>
       <c r="H57" s="13" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="I57" s="6"/>
       <c r="J57" s="18"/>
@@ -3711,37 +3753,71 @@
       <c r="A58" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B58" s="6"/>
-      <c r="C58" s="6"/>
-      <c r="D58" s="6"/>
-      <c r="E58" s="12"/>
-      <c r="F58" s="6"/>
+      <c r="B58" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>416</v>
+      </c>
+      <c r="E58" s="12" t="s">
+        <v>417</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>129</v>
+      </c>
       <c r="G58" s="6"/>
       <c r="H58" s="13" t="s">
-        <v>336</v>
-      </c>
-      <c r="I58" s="6"/>
-      <c r="J58" s="18"/>
-      <c r="K58" s="6"/>
-      <c r="L58" s="22"/>
+        <v>334</v>
+      </c>
+      <c r="I58" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="J58" s="18">
+        <v>0</v>
+      </c>
+      <c r="K58" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="L58" s="22">
+        <v>0</v>
+      </c>
       <c r="M58" s="6"/>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B59" s="6"/>
-      <c r="C59" s="6"/>
-      <c r="D59" s="6"/>
-      <c r="E59" s="12"/>
-      <c r="F59" s="6"/>
+      <c r="B59" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="E59" s="12" t="s">
+        <v>419</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>420</v>
+      </c>
       <c r="G59" s="6"/>
       <c r="H59" s="13" t="s">
-        <v>337</v>
-      </c>
-      <c r="I59" s="6"/>
-      <c r="J59" s="18"/>
-      <c r="K59" s="6"/>
+        <v>335</v>
+      </c>
+      <c r="I59" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="J59" s="18" t="s">
+        <v>421</v>
+      </c>
+      <c r="K59" s="6" t="s">
+        <v>235</v>
+      </c>
       <c r="L59" s="22"/>
       <c r="M59" s="6"/>
     </row>
@@ -3749,14 +3825,20 @@
       <c r="A60" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B60" s="6"/>
-      <c r="C60" s="6"/>
-      <c r="D60" s="6"/>
+      <c r="B60" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>422</v>
+      </c>
       <c r="E60" s="12"/>
       <c r="F60" s="6"/>
       <c r="G60" s="13"/>
       <c r="H60" s="13" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="I60" s="6"/>
       <c r="J60" s="18"/>
@@ -3775,7 +3857,7 @@
       <c r="F61" s="6"/>
       <c r="G61" s="6"/>
       <c r="H61" s="13" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="I61" s="6"/>
       <c r="J61" s="18"/>
@@ -3794,7 +3876,7 @@
       <c r="F62" s="6"/>
       <c r="G62" s="6"/>
       <c r="H62" s="13" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="I62" s="6"/>
       <c r="J62" s="18"/>
@@ -3813,7 +3895,7 @@
       <c r="F63" s="6"/>
       <c r="G63" s="6"/>
       <c r="H63" s="13" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="I63" s="6"/>
       <c r="J63" s="18"/>
@@ -3832,7 +3914,7 @@
       <c r="F64" s="6"/>
       <c r="G64" s="6"/>
       <c r="H64" s="13" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="I64" s="6"/>
       <c r="J64" s="18"/>
@@ -3851,7 +3933,7 @@
       <c r="F65" s="6"/>
       <c r="G65" s="13"/>
       <c r="H65" s="13" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="I65" s="6"/>
       <c r="J65" s="18"/>
@@ -3870,7 +3952,7 @@
       <c r="F66" s="6"/>
       <c r="G66" s="13"/>
       <c r="H66" s="13" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="I66" s="6"/>
       <c r="J66" s="18"/>
@@ -3889,7 +3971,7 @@
       <c r="F67" s="6"/>
       <c r="G67" s="6"/>
       <c r="H67" s="13" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="I67" s="6"/>
       <c r="J67" s="18"/>
@@ -3899,7 +3981,7 @@
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
@@ -3908,7 +3990,7 @@
       <c r="F68" s="6"/>
       <c r="G68" s="6"/>
       <c r="H68" s="13" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="I68" s="6"/>
       <c r="J68" s="18"/>
@@ -3927,7 +4009,7 @@
       <c r="F69" s="6"/>
       <c r="G69" s="6"/>
       <c r="H69" s="13" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="I69" s="6"/>
       <c r="J69" s="18"/>
@@ -3946,7 +4028,7 @@
       <c r="F70" s="6"/>
       <c r="G70" s="6"/>
       <c r="H70" s="13" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="I70" s="6"/>
       <c r="J70" s="18"/>
@@ -3965,7 +4047,7 @@
       <c r="F71" s="6"/>
       <c r="G71" s="6"/>
       <c r="H71" s="13" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="I71" s="6"/>
       <c r="J71" s="18"/>
@@ -3984,7 +4066,7 @@
       <c r="F72" s="6"/>
       <c r="G72" s="6"/>
       <c r="H72" s="13" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="I72" s="6"/>
       <c r="J72" s="18"/>
@@ -4003,7 +4085,7 @@
       <c r="F73" s="6"/>
       <c r="G73" s="6"/>
       <c r="H73" s="13" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="I73" s="6"/>
       <c r="J73" s="18"/>
@@ -4022,7 +4104,7 @@
       <c r="F74" s="6"/>
       <c r="G74" s="6"/>
       <c r="H74" s="13" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="I74" s="6"/>
       <c r="J74" s="18"/>
@@ -4041,7 +4123,7 @@
       <c r="F75" s="6"/>
       <c r="G75" s="6"/>
       <c r="H75" s="13" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="I75" s="6"/>
       <c r="J75" s="18"/>
@@ -4060,7 +4142,7 @@
       <c r="F76" s="6"/>
       <c r="G76" s="6"/>
       <c r="H76" s="13" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="I76" s="6"/>
       <c r="J76" s="18"/>
@@ -4079,7 +4161,7 @@
       <c r="F77" s="6"/>
       <c r="G77" s="6"/>
       <c r="H77" s="13" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="I77" s="6"/>
       <c r="J77" s="18"/>
@@ -4098,7 +4180,7 @@
       <c r="F78" s="6"/>
       <c r="G78" s="6"/>
       <c r="H78" s="13" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="I78" s="6"/>
       <c r="J78" s="18"/>
@@ -4117,7 +4199,7 @@
       <c r="F79" s="6"/>
       <c r="G79" s="6"/>
       <c r="H79" s="13" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="I79" s="6"/>
       <c r="J79" s="18"/>
@@ -4136,7 +4218,7 @@
       <c r="F80" s="6"/>
       <c r="G80" s="6"/>
       <c r="H80" s="13" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="I80" s="6"/>
       <c r="J80" s="18"/>
@@ -4155,7 +4237,7 @@
       <c r="F81" s="6"/>
       <c r="G81" s="6"/>
       <c r="H81" s="13" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="I81" s="6"/>
       <c r="J81" s="18"/>
@@ -4174,7 +4256,7 @@
       <c r="F82" s="6"/>
       <c r="G82" s="6"/>
       <c r="H82" s="13" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="I82" s="6"/>
       <c r="J82" s="18"/>
@@ -4193,7 +4275,7 @@
       <c r="F83" s="6"/>
       <c r="G83" s="6"/>
       <c r="H83" s="13" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="I83" s="6"/>
       <c r="J83" s="18"/>
@@ -4212,7 +4294,7 @@
       <c r="F84" s="6"/>
       <c r="G84" s="6"/>
       <c r="H84" s="13" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I84" s="6"/>
       <c r="J84" s="18"/>
@@ -4231,7 +4313,7 @@
       <c r="F85" s="6"/>
       <c r="G85" s="6"/>
       <c r="H85" s="13" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="I85" s="6"/>
       <c r="J85" s="18"/>
@@ -4250,7 +4332,7 @@
       <c r="F86" s="6"/>
       <c r="G86" s="6"/>
       <c r="H86" s="13" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="I86" s="6"/>
       <c r="J86" s="18"/>
@@ -4269,7 +4351,7 @@
       <c r="F87" s="6"/>
       <c r="G87" s="6"/>
       <c r="H87" s="13" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="I87" s="6"/>
       <c r="J87" s="18"/>
@@ -4288,7 +4370,7 @@
       <c r="F88" s="6"/>
       <c r="G88" s="13"/>
       <c r="H88" s="13" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="I88" s="6"/>
       <c r="J88" s="18"/>
@@ -4307,7 +4389,7 @@
       <c r="F89" s="6"/>
       <c r="G89" s="6"/>
       <c r="H89" s="13" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="I89" s="6"/>
       <c r="J89" s="18"/>
@@ -4326,7 +4408,7 @@
       <c r="F90" s="6"/>
       <c r="G90" s="6"/>
       <c r="H90" s="13" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="I90" s="6"/>
       <c r="J90" s="18"/>
@@ -4345,7 +4427,7 @@
       <c r="F91" s="6"/>
       <c r="G91" s="6"/>
       <c r="H91" s="13" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="I91" s="6"/>
       <c r="J91" s="18"/>
@@ -4364,7 +4446,7 @@
       <c r="F92" s="6"/>
       <c r="G92" s="6"/>
       <c r="H92" s="13" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="I92" s="6"/>
       <c r="J92" s="18"/>
@@ -4383,7 +4465,7 @@
       <c r="F93" s="6"/>
       <c r="G93" s="6"/>
       <c r="H93" s="13" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="I93" s="6"/>
       <c r="J93" s="18"/>
@@ -4402,7 +4484,7 @@
       <c r="F94" s="6"/>
       <c r="G94" s="6"/>
       <c r="H94" s="13" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="I94" s="6"/>
       <c r="J94" s="18"/>
@@ -4579,11 +4661,12 @@
     <hyperlink ref="I54" r:id="rId87"/>
     <hyperlink ref="H55" r:id="rId88"/>
     <hyperlink ref="I55" r:id="rId89"/>
+    <hyperlink ref="I28" r:id="rId90"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId90"/>
+  <pageSetup orientation="portrait" r:id="rId91"/>
   <tableParts count="1">
-    <tablePart r:id="rId91"/>
+    <tablePart r:id="rId92"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -4892,6 +4975,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100195A0DC3D759E3489DFA9C5205E5B14C" ma:contentTypeVersion="2" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="50d30e209eacd544e519b0de95956bf8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9557b78e-b540-44eb-8496-d55148e88a38" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="093a042629348530cc8d8a9fb023c1bd" ns2:_="">
     <xsd:import namespace="9557b78e-b540-44eb-8496-d55148e88a38"/>
@@ -5023,12 +5112,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{723C7C72-FB82-4CAD-AEF8-0F96687F8D2E}">
   <ds:schemaRefs>
@@ -5038,6 +5121,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE39B8A0-603B-4CD4-BED2-FB7318812FE6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9557b78e-b540-44eb-8496-d55148e88a38"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD7DD402-3AFE-43B9-82AA-89DC3E0E2BD0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5053,20 +5152,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE39B8A0-603B-4CD4-BED2-FB7318812FE6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9557b78e-b540-44eb-8496-d55148e88a38"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
part 1 rapport final
</commit_message>
<xml_diff>
--- a/Electronic/Components/Electronics-Components-Index.xlsx
+++ b/Electronic/Components/Electronics-Components-Index.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emile\6DOF-Robotic-Arm\Electronic\Components\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SDD Files\Documents\6DOF-Robotic-Arm\Electronic\Components\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1311,8 +1311,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -1386,7 +1386,7 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1415,7 +1415,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1424,20 +1424,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1463,7 +1463,7 @@
   </cellStyles>
   <dxfs count="14">
     <dxf>
-      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+      <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1932,8 +1932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4689,11 +4689,12 @@
     <hyperlink ref="H55" r:id="rId88"/>
     <hyperlink ref="I55" r:id="rId89"/>
     <hyperlink ref="I28" r:id="rId90"/>
+    <hyperlink ref="H59" r:id="rId91"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId91"/>
+  <pageSetup orientation="portrait" r:id="rId92"/>
   <tableParts count="1">
-    <tablePart r:id="rId92"/>
+    <tablePart r:id="rId93"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -5002,6 +5003,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100195A0DC3D759E3489DFA9C5205E5B14C" ma:contentTypeVersion="2" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="50d30e209eacd544e519b0de95956bf8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9557b78e-b540-44eb-8496-d55148e88a38" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="093a042629348530cc8d8a9fb023c1bd" ns2:_="">
     <xsd:import namespace="9557b78e-b540-44eb-8496-d55148e88a38"/>
@@ -5133,12 +5140,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{723C7C72-FB82-4CAD-AEF8-0F96687F8D2E}">
   <ds:schemaRefs>
@@ -5148,6 +5149,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE39B8A0-603B-4CD4-BED2-FB7318812FE6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9557b78e-b540-44eb-8496-d55148e88a38"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD7DD402-3AFE-43B9-82AA-89DC3E0E2BD0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5163,20 +5180,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE39B8A0-603B-4CD4-BED2-FB7318812FE6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9557b78e-b540-44eb-8496-d55148e88a38"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>